<commit_message>
Add calc U I angles
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Уст. Знач:</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Binom#</t>
+  </si>
+  <si>
+    <t>freq</t>
   </si>
 </sst>
 </file>
@@ -574,133 +577,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI13"/>
+  <dimension ref="A1:AJ13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AG1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AH1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AI1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -736,28 +742,29 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ3" s="1"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -793,22 +800,23 @@
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ8" s="1"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Repair template and make some works on report
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -36,15 +36,6 @@
     <t>Uc</t>
   </si>
   <si>
-    <t>AngleUab</t>
-  </si>
-  <si>
-    <t>AngleUbc</t>
-  </si>
-  <si>
-    <t>AngleUca</t>
-  </si>
-  <si>
     <t>Ia</t>
   </si>
   <si>
@@ -90,9 +81,6 @@
     <t>Pc</t>
   </si>
   <si>
-    <t>Pabc</t>
-  </si>
-  <si>
     <t>Qa</t>
   </si>
   <si>
@@ -102,9 +90,6 @@
     <t>Qc</t>
   </si>
   <si>
-    <t>Qabc</t>
-  </si>
-  <si>
     <t>Sa</t>
   </si>
   <si>
@@ -112,18 +97,6 @@
   </si>
   <si>
     <t>Sc</t>
-  </si>
-  <si>
-    <t>Sabc</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>S1</t>
   </si>
   <si>
     <t>Эталон MTE</t>
@@ -186,6 +159,33 @@
   </si>
   <si>
     <t>freq</t>
+  </si>
+  <si>
+    <t>AngUab</t>
+  </si>
+  <si>
+    <t>AngUbc</t>
+  </si>
+  <si>
+    <t>AngUca</t>
+  </si>
+  <si>
+    <t>AngIab</t>
+  </si>
+  <si>
+    <t>AngIbc</t>
+  </si>
+  <si>
+    <t>AngIca</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A1:AJ13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,9 +589,9 @@
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -599,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>2</v>
@@ -611,94 +611,94 @@
         <v>4</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="M1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AG1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="AH1" s="7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="AI1" s="7" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="AJ1" s="7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -746,22 +746,22 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
@@ -804,7 +804,7 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
start work on report
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Уст. Знач:</t>
   </si>
@@ -186,6 +186,15 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Binom Δ изм</t>
+  </si>
+  <si>
+    <t>Binom δ изм</t>
+  </si>
+  <si>
+    <t>Binom γ изм</t>
   </si>
 </sst>
 </file>
@@ -580,7 +589,7 @@
   <dimension ref="A1:AJ13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ2" sqref="AJ2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,21 +812,62 @@
       <c r="AJ8" s="1"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>